<commit_message>
Updated page #s of PRISMA checklist.
</commit_message>
<xml_diff>
--- a/prisma.xlsx
+++ b/prisma.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t xml:space="preserve">Section </t>
   </si>
@@ -79,6 +79,9 @@
     <t xml:space="preserve">Indicate if a review protocol exists, if and where it can be accessed (e.g., Web address), and, if available, provide registration information including registration number. </t>
   </si>
   <si>
+    <t xml:space="preserve">Not applicable</t>
+  </si>
+  <si>
     <t xml:space="preserve">Eligibility criteria </t>
   </si>
   <si>
@@ -177,9 +180,6 @@
   </si>
   <si>
     <t xml:space="preserve">Describe methods used for assessing risk of bias of individual studies (including specification of whether this was done at the study or outcome level), and how this information is to be used in any data synthesis. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not applicable</t>
   </si>
   <si>
     <t xml:space="preserve">Summary measures </t>
@@ -368,7 +368,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -392,7 +392,7 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -400,7 +400,7 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -408,13 +408,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -514,11 +507,15 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -551,20 +548,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -647,418 +636,454 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="3.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="238.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.16"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="3.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="238.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="9"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="E2" s="10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="E3" s="10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="10" t="n">
+      <c r="C4" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11"/>
-      <c r="B5" s="6" t="s">
+      <c r="E4" s="10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="E5" s="10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="10" t="n">
+      <c r="C6" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12"/>
-      <c r="B7" s="8" t="s">
+      <c r="E6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="10" t="n">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="11" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="11" t="n">
+        <v>11</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="11" t="n">
+        <v>12</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="11" t="n">
+        <v>13</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="11" t="n">
+        <v>14</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="8" t="n">
+        <v>16</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="11" t="n">
+        <v>17</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="10" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="11" t="n">
+        <v>18</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="10" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="11" t="n">
+        <v>19</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12"/>
-      <c r="B8" s="8" t="s">
+      <c r="D21" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="11" t="n">
         <v>21</v>
       </c>
-      <c r="C8" s="10" t="n">
+      <c r="D22" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="10" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="11" t="n">
+        <v>22</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="8" t="n">
+        <v>23</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="11" t="n">
+        <v>24</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12"/>
-      <c r="B9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="10" t="n">
-        <v>8</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12"/>
-      <c r="B10" s="8" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="11" t="n">
         <v>25</v>
       </c>
-      <c r="C10" s="10" t="n">
-        <v>9</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="D26" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="10" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="8" t="n">
         <v>26</v>
       </c>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12"/>
-      <c r="B11" s="8" t="s">
+      <c r="D27" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="10" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="11" t="n">
         <v>27</v>
       </c>
-      <c r="C11" s="10" t="n">
+      <c r="D28" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12"/>
-      <c r="B12" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12"/>
-      <c r="B13" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="10" t="n">
-        <v>12</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12"/>
-      <c r="B14" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="10" t="n">
-        <v>13</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12"/>
-      <c r="B15" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="10" t="n">
-        <v>14</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12"/>
-      <c r="B16" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="10" t="n">
-        <v>15</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11"/>
-      <c r="B17" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="7" t="n">
-        <v>16</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="10" t="n">
-        <v>17</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12"/>
-      <c r="B19" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="10" t="n">
-        <v>18</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12"/>
-      <c r="B20" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="10" t="n">
-        <v>19</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12"/>
-      <c r="B21" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12"/>
-      <c r="B22" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="10" t="n">
-        <v>21</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12"/>
-      <c r="B23" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="10" t="n">
-        <v>22</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11"/>
-      <c r="B24" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="7" t="n">
-        <v>23</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="10" t="n">
-        <v>24</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="9"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12"/>
-      <c r="B26" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="10" t="n">
-        <v>25</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="9"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11"/>
-      <c r="B27" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="7" t="n">
-        <v>26</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="9"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="10" t="n">
-        <v>27</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>